<commit_message>
Ready for GenA talk
</commit_message>
<xml_diff>
--- a/HowTo.xlsx
+++ b/HowTo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cliff\OneDrive\Documents\GenAtomic\Optimize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E107336B-0C9C-4FAA-8F9C-72677E692770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED16E51-27CA-4E7A-9893-06E986334EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{D1AEF0B0-29D5-4C22-9FE1-30CC505B8A1D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>Step 1:</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>HowTo.xlsx</t>
-  </si>
-  <si>
-    <t>You have downloaded the entire directory CCL_Shared as a Compressed (Zipped) file</t>
   </si>
   <si>
     <r>
@@ -113,9 +110,6 @@
     <t>This File Link:</t>
   </si>
   <si>
-    <t>Copy zip file from your download directory to your desired Target directory.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Close This File, Open </t>
     </r>
@@ -167,9 +161,6 @@
     </r>
   </si>
   <si>
-    <t>When you Ctrl-Click on C3, a new Browser Tab will appear.  Click on the Tab, and then click on Download in that Tab. Then Close Tab.  Ctrl-Click C3 now.</t>
-  </si>
-  <si>
     <t>If required, complete Phase 2</t>
   </si>
   <si>
@@ -189,6 +180,12 @@
   </si>
   <si>
     <t>Step 9:</t>
+  </si>
+  <si>
+    <t>Wait until you have downloaded the entire directory CCL_Shared as a Compressed (Zipped) file</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <r>
@@ -210,8 +207,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Print a copy of this, but leave this window open.  Use the File menu at the left to print.</t>
+      <t>Print a copy of this, but leave this window open.  Use the "File" menu at the left to print.</t>
     </r>
+  </si>
+  <si>
+    <t>Close the browser.  Copy zip file from your download directory to your desired Target directory.</t>
+  </si>
+  <si>
+    <t>When you Click on C4, a new Browser Tab will appear.  Click on the Tab, and then click on Download (Upper Left).  Click C4 now.</t>
   </si>
 </sst>
 </file>
@@ -257,11 +260,63 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -270,17 +325,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -617,189 +697,251 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5B33D7-FCCA-4080-A2B8-E9ECEEDA5CF3}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
   <cols>
+    <col min="2" max="2" width="8.921875" style="4"/>
+    <col min="3" max="3" width="56.765625" customWidth="1"/>
     <col min="12" max="12" width="8.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.85">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34.299999999999997" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="38.15" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="B3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.85">
+      <c r="B4" s="12"/>
+      <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="29.15" x14ac:dyDescent="0.85">
+      <c r="B5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29.15" x14ac:dyDescent="0.85">
+      <c r="B6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.85">
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29.15" x14ac:dyDescent="0.85">
+      <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.85">
-      <c r="B2" t="s">
+      <c r="C8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="29.15" x14ac:dyDescent="0.85">
+      <c r="B9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="28.3" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="B3" s="2" t="s">
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.85">
+      <c r="B10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.85">
+      <c r="B11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.85">
+      <c r="B12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.85">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.85">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.85">
+      <c r="B15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="29.15" x14ac:dyDescent="0.85">
+      <c r="B16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
-      <c r="B6" t="s">
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.85">
+      <c r="B17" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
-      <c r="B7" t="s">
+      <c r="C17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.85">
+      <c r="B18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
-      <c r="B9" t="s">
+      <c r="C18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.85">
+      <c r="B19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.85">
+      <c r="B20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
-      <c r="B10" t="s">
+      <c r="C20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.85">
+      <c r="B21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="14.65" x14ac:dyDescent="0.85"/>
-    <row r="14" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.85">
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.85">
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.85">
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.85">
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.85">
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>18</v>
+      <c r="C21" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.85">
+      <c r="D22" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C3:L3"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" display="https://1drv.ms/f/s!ApcqMlOg59B8g78LLkCsqNJ86gfqsg?e=3iOC3l" xr:uid="{62C7ABCC-C39F-4E18-8D68-837DCDB60954}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -816,7 +958,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.85">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>

</xml_diff>